<commit_message>
EBO App Factory documentation updated
</commit_message>
<xml_diff>
--- a/ebo_app_factory/examples/basic apps example.xlsx
+++ b/ebo_app_factory/examples/basic apps example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sesa368046\Documents\Solutions\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F635414-B406-4229-9FE8-632042632C38}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D35B7E5-F34B-488F-BA7B-1FDC9A9F9537}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1275" yWindow="-120" windowWidth="27645" windowHeight="16440" xr2:uid="{34A6D1F0-A03F-41DF-A80D-622D97479DCE}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>VAV-L16-INT1</t>
   </si>
@@ -63,6 +63,18 @@
   </si>
   <si>
     <t>L21-INT4</t>
+  </si>
+  <si>
+    <t>VAV-L21-NW2</t>
+  </si>
+  <si>
+    <t>L21-NW2</t>
+  </si>
+  <si>
+    <t>VAV-L04-INT09</t>
+  </si>
+  <si>
+    <t>L04_INT09</t>
   </si>
 </sst>
 </file>
@@ -414,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2BFABE1-FBEF-4404-9EDF-8937AFE2CC23}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -466,6 +478,22 @@
         <v>8</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>